<commit_message>
Blur the edge of each cell
Use medianBlur function in OpenCV to blur the edge of each cell. The
human eye result is much better and the SSIM value is higher.
</commit_message>
<xml_diff>
--- a/Experiments/MakeGraph.xlsx
+++ b/Experiments/MakeGraph.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t>SSIM</t>
   </si>
@@ -79,6 +79,51 @@
   </si>
   <si>
     <t>head1080_cells20_20</t>
+  </si>
+  <si>
+    <t>num_PCA</t>
+  </si>
+  <si>
+    <t>head720_cells10_19</t>
+  </si>
+  <si>
+    <t>head720_cells10_16</t>
+  </si>
+  <si>
+    <t>head720_cells10_13</t>
+  </si>
+  <si>
+    <t>head720_cells10_10</t>
+  </si>
+  <si>
+    <t>head720_cells10_7</t>
+  </si>
+  <si>
+    <t>head720_cells5_7</t>
+  </si>
+  <si>
+    <t>head720_cells5_6</t>
+  </si>
+  <si>
+    <t>head720_cells5_5</t>
+  </si>
+  <si>
+    <t>head720_cells5_4</t>
+  </si>
+  <si>
+    <t>head720_cells5_8</t>
+  </si>
+  <si>
+    <t>head720_cells30_65</t>
+  </si>
+  <si>
+    <t>head720_cells30_70</t>
+  </si>
+  <si>
+    <t>head720_cells30_75</t>
+  </si>
+  <si>
+    <t>head720_cells30_80</t>
   </si>
 </sst>
 </file>
@@ -179,7 +224,16 @@
               <a:rPr lang="en-US" sz="2800" b="1" baseline="0"/>
               <a:t> Dimension</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US" sz="2800" b="1"/>
+          </a:p>
+          <a:p>
+            <a:pPr algn="ctr">
+              <a:defRPr b="1"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" baseline="0"/>
+              <a:t>(Top figure of each point is the number of eigenvectors)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1800" b="1"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -227,8 +281,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0545012328132887"/>
-          <c:y val="0.158941015927414"/>
+          <c:x val="0.0535226509438128"/>
+          <c:y val="0.158941069198084"/>
           <c:w val="0.799237104718402"/>
           <c:h val="0.749367546465996"/>
         </c:manualLayout>
@@ -237,8 +291,88 @@
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Re:720/Cell:10</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$24:$B$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.977</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.973</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.968</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.946</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$24:$C$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:v>Re:720/Cell:20</c:v>
           </c:tx>
@@ -266,68 +400,9 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="t"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$10:$B$14</c:f>
+              <c:f>Sheet1!$B$16:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -351,7 +426,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$10:$C$14</c:f>
+              <c:f>Sheet1!$C$16:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -368,7 +443,7 @@
                   <c:v>11.9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14.0</c:v>
+                  <c:v>12.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -377,7 +452,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:v>Re:720/Cell:30</c:v>
           </c:tx>
@@ -406,68 +481,9 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="t"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$6</c:f>
+              <c:f>Sheet1!$B$6:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -491,7 +507,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$6</c:f>
+              <c:f>Sheet1!$C$6:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -517,7 +533,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:v>Re:1080/Cell:20</c:v>
           </c:tx>
@@ -545,68 +561,9 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="t"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$18:$B$22</c:f>
+              <c:f>Sheet1!$B$40:$B$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -630,7 +587,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$18:$C$22</c:f>
+              <c:f>Sheet1!$C$40:$C$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -655,19 +612,18 @@
           <c:smooth val="1"/>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
+          <c:showVal val="0"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1940586816"/>
-        <c:axId val="-2030278928"/>
+        <c:axId val="-594085056"/>
+        <c:axId val="-554766416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1940586816"/>
+        <c:axId val="-594085056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -736,6 +692,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -772,12 +729,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2030278928"/>
+        <c:crossAx val="-554766416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2030278928"/>
+        <c:axId val="-554766416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -898,7 +855,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1940586816"/>
+        <c:crossAx val="-594085056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -912,29 +869,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:legendEntry>
-        <c:idx val="0"/>
-        <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-      </c:legendEntry>
       <c:legendEntry>
         <c:idx val="1"/>
         <c:txPr>
@@ -981,14 +915,37 @@
           </a:p>
         </c:txPr>
       </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="3"/>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.836572625867975"/>
           <c:y val="0.368044087178682"/>
-          <c:w val="0.161950090031529"/>
-          <c:h val="0.268409735146743"/>
+          <c:w val="0.120069691045029"/>
+          <c:h val="0.182969698283488"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1004,7 +961,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1054,6 +1011,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -1247,7 +1205,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1268,7 +1225,7 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$6</c:f>
+              <c:f>Sheet1!$B$6:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1292,7 +1249,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$6</c:f>
+              <c:f>Sheet1!$C$6:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1325,11 +1282,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1938515328"/>
-        <c:axId val="-1913052912"/>
+        <c:axId val="-594563584"/>
+        <c:axId val="-594561040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1938515328"/>
+        <c:axId val="-594563584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1434,12 +1391,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1913052912"/>
+        <c:crossAx val="-594561040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1913052912"/>
+        <c:axId val="-594561040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -1500,7 +1457,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1560,7 +1516,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1938515328"/>
+        <c:crossAx val="-594563584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2699,20 +2655,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>634999</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>75596</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>225777</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>14111</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>423332</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>820904</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>52366</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="10" name="Chart 9"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -2733,6 +2689,871 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.1596</cdr:x>
+      <cdr:y>0.21777</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.18749</cdr:x>
+      <cdr:y>0.24738</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2071237" y="1601386"/>
+          <a:ext cx="362002" cy="217708"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>40</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.00391</cdr:x>
+      <cdr:y>0.00691</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.03181</cdr:x>
+      <cdr:y>0.03651</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 2"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="50800" y="50800"/>
+          <a:ext cx="362002" cy="217708"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.25501</cdr:x>
+      <cdr:y>0.24402</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.28328</cdr:x>
+      <cdr:y>0.27027</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="5" name="TextBox 4"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3299743" y="1794369"/>
+          <a:ext cx="365760" cy="193040"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>45</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.32489</cdr:x>
+      <cdr:y>0.27027</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.35002</cdr:x>
+      <cdr:y>0.30067</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="6" name="TextBox 5"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="4203983" y="1987409"/>
+          <a:ext cx="325120" cy="223520"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>50</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.37279</cdr:x>
+      <cdr:y>0.29928</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.39949</cdr:x>
+      <cdr:y>0.33106</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="7" name="TextBox 6"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="4823743" y="2200769"/>
+          <a:ext cx="345440" cy="233680"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>55</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.43011</cdr:x>
+      <cdr:y>0.31586</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.45602</cdr:x>
+      <cdr:y>0.34764</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="8" name="TextBox 7"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="5565423" y="2322689"/>
+          <a:ext cx="335280" cy="233680"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>60</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.23146</cdr:x>
+      <cdr:y>0.3283</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.25423</cdr:x>
+      <cdr:y>0.35731</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="9" name="TextBox 8"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2994943" y="2414129"/>
+          <a:ext cx="294640" cy="213360"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.22441</cdr:x>
+      <cdr:y>0.33866</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.25622</cdr:x>
+      <cdr:y>0.36406</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="10" name="TextBox 9"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2921614" y="2503802"/>
+          <a:ext cx="414131" cy="187739"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>20</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.37201</cdr:x>
+      <cdr:y>0.38123</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.40339</cdr:x>
+      <cdr:y>0.40887</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="11" name="TextBox 10"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="4843179" y="2818541"/>
+          <a:ext cx="408609" cy="204304"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>25</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.48147</cdr:x>
+      <cdr:y>0.41014</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.514</cdr:x>
+      <cdr:y>0.43903</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="12" name="TextBox 11"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="6265333" y="3071518"/>
+          <a:ext cx="423334" cy="216370"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>30</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.56172</cdr:x>
+      <cdr:y>0.4629</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.59931</cdr:x>
+      <cdr:y>0.48928</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="13" name="TextBox 12"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="7309556" y="3466630"/>
+          <a:ext cx="489185" cy="197555"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>35</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.61738</cdr:x>
+      <cdr:y>0.47923</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.64341</cdr:x>
+      <cdr:y>0.51692</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="14" name="TextBox 13"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="8033927" y="3588926"/>
+          <a:ext cx="338666" cy="282222"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>40</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.3891</cdr:x>
+      <cdr:y>0.35616</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.42092</cdr:x>
+      <cdr:y>0.38149</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="15" name="TextBox 14"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="5074357" y="2619022"/>
+          <a:ext cx="414866" cy="186266"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>7</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.57543</cdr:x>
+      <cdr:y>0.36652</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.60789</cdr:x>
+      <cdr:y>0.39416</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="16" name="TextBox 15"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="7504290" y="2695222"/>
+          <a:ext cx="423333" cy="203200"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.57543</cdr:x>
+      <cdr:y>0.36422</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.60465</cdr:x>
+      <cdr:y>0.39646</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="18" name="TextBox 17"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="7504290" y="2678289"/>
+          <a:ext cx="381000" cy="237067"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>10</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.68061</cdr:x>
+      <cdr:y>0.3907</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.71112</cdr:x>
+      <cdr:y>0.42179</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="19" name="TextBox 18"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="8875890" y="2873022"/>
+          <a:ext cx="397933" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>13</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.74683</cdr:x>
+      <cdr:y>0.42409</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.78124</cdr:x>
+      <cdr:y>0.44827</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="20" name="TextBox 19"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="9739490" y="3118555"/>
+          <a:ext cx="448734" cy="177800"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>16</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.80266</cdr:x>
+      <cdr:y>0.45288</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.82993</cdr:x>
+      <cdr:y>0.48051</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="21" name="TextBox 20"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="10467624" y="3330223"/>
+          <a:ext cx="355600" cy="203200"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>19</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.44001</cdr:x>
+      <cdr:y>0.61353</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.46899</cdr:x>
+      <cdr:y>0.65372</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="22" name="TextBox 21"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="5728498" y="4495309"/>
+          <a:ext cx="377319" cy="294493"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>20</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.54816</cdr:x>
+      <cdr:y>0.64493</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.57785</cdr:x>
+      <cdr:y>0.68136</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="23" name="TextBox 22"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="7136541" y="4725382"/>
+          <a:ext cx="386522" cy="266884"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>25</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.6139</cdr:x>
+      <cdr:y>0.65624</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.64218</cdr:x>
+      <cdr:y>0.68889</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="24" name="TextBox 23"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="7992411" y="4808208"/>
+          <a:ext cx="368116" cy="239275"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>30</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.66692</cdr:x>
+      <cdr:y>0.68512</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.70014</cdr:x>
+      <cdr:y>0.71653</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="25" name="TextBox 24"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="8682629" y="5019874"/>
+          <a:ext cx="432536" cy="230073"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>35</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.72135</cdr:x>
+      <cdr:y>0.69517</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.74962</cdr:x>
+      <cdr:y>0.7316</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="26" name="TextBox 25"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="9391252" y="5093498"/>
+          <a:ext cx="368116" cy="266884"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>40</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3032,10 +3853,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" zoomScale="84" workbookViewId="0">
-      <selection activeCell="U12" sqref="U12"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="89" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3043,193 +3864,426 @@
     <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="B6">
         <v>0.94899999999999995</v>
       </c>
-      <c r="C2">
+      <c r="C6">
         <v>13.3</v>
       </c>
+      <c r="D6">
+        <v>60</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="B7">
         <v>0.94499999999999995</v>
       </c>
-      <c r="C3">
+      <c r="C7">
         <v>13.8</v>
       </c>
+      <c r="D7">
+        <v>55</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="B8">
         <v>0.94099999999999995</v>
       </c>
-      <c r="C4">
+      <c r="C8">
         <v>14.5</v>
       </c>
+      <c r="D8">
+        <v>50</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
+      <c r="B9">
         <v>0.93600000000000005</v>
       </c>
-      <c r="C5">
+      <c r="C9">
         <v>15.1</v>
       </c>
+      <c r="D9">
+        <v>45</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
+      <c r="B10">
         <v>0.92900000000000005</v>
       </c>
-      <c r="C6">
+      <c r="C10">
         <v>15.7</v>
       </c>
+      <c r="D10">
+        <v>40</v>
+      </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
         <v>0</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C15" t="s">
         <v>1</v>
       </c>
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>7</v>
       </c>
-      <c r="B10">
+      <c r="B16">
         <v>0.96299999999999997</v>
       </c>
-      <c r="C10">
+      <c r="C16">
         <v>9.5</v>
       </c>
+      <c r="D16">
+        <v>40</v>
+      </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>8</v>
       </c>
-      <c r="B11">
+      <c r="B17">
         <v>0.95899999999999996</v>
       </c>
-      <c r="C11">
+      <c r="C17">
         <v>10</v>
       </c>
+      <c r="D17">
+        <v>35</v>
+      </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>9</v>
       </c>
-      <c r="B12">
+      <c r="B18">
         <v>0.95299999999999996</v>
       </c>
-      <c r="C12">
+      <c r="C18">
         <v>11.2</v>
       </c>
+      <c r="D18">
+        <v>30</v>
+      </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>10</v>
       </c>
-      <c r="B13">
+      <c r="B19">
         <v>0.94499999999999995</v>
       </c>
-      <c r="C13">
+      <c r="C19">
         <v>11.9</v>
       </c>
+      <c r="D19">
+        <v>25</v>
+      </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>11</v>
       </c>
-      <c r="B14">
+      <c r="B20">
         <v>0.93400000000000005</v>
       </c>
-      <c r="C14">
+      <c r="C20">
+        <v>12.9</v>
+      </c>
+      <c r="D20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24">
+        <v>0.97699999999999998</v>
+      </c>
+      <c r="C24">
+        <v>10.1</v>
+      </c>
+      <c r="D24">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25">
+        <v>0.97299999999999998</v>
+      </c>
+      <c r="C25">
+        <v>10.7</v>
+      </c>
+      <c r="D25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26">
+        <v>0.96799999999999997</v>
+      </c>
+      <c r="C26">
+        <v>11.5</v>
+      </c>
+      <c r="D26">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27">
+        <v>0.96</v>
+      </c>
+      <c r="C27">
+        <v>12.2</v>
+      </c>
+      <c r="D27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28">
+        <v>0.94599999999999995</v>
+      </c>
+      <c r="C28">
+        <v>13.3</v>
+      </c>
+      <c r="D28">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32">
+        <v>7.28</v>
+      </c>
+      <c r="D32">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33">
+        <v>7.48</v>
+      </c>
+      <c r="D33">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34">
+        <v>7.29</v>
+      </c>
+      <c r="D34">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35">
+        <v>7.35</v>
+      </c>
+      <c r="D35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36">
+        <v>7.33</v>
+      </c>
+      <c r="D36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40">
+        <v>0.97099999999999997</v>
+      </c>
+      <c r="C40">
+        <v>4.3</v>
+      </c>
+      <c r="D40">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41">
+        <v>0.96699999999999997</v>
+      </c>
+      <c r="C41">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D41">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>14</v>
       </c>
+      <c r="B42">
+        <v>0.96299999999999997</v>
+      </c>
+      <c r="C42">
+        <v>5.2</v>
+      </c>
+      <c r="D42">
+        <v>30</v>
+      </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" t="s">
-        <v>1</v>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>15</v>
+      </c>
+      <c r="B43">
+        <v>0.95799999999999996</v>
+      </c>
+      <c r="C43">
+        <v>5.5</v>
+      </c>
+      <c r="D43">
+        <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18">
-        <v>0.97099999999999997</v>
-      </c>
-      <c r="C18">
-        <v>4.3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19">
-        <v>0.96699999999999997</v>
-      </c>
-      <c r="C19">
-        <v>4.5999999999999996</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20">
-        <v>0.96299999999999997</v>
-      </c>
-      <c r="C20">
-        <v>5.2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21">
-        <v>0.95799999999999996</v>
-      </c>
-      <c r="C21">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>16</v>
       </c>
-      <c r="B22">
+      <c r="B44">
         <v>0.95</v>
       </c>
-      <c r="C22">
+      <c r="C44">
         <v>6.2</v>
+      </c>
+      <c r="D44">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -3243,7 +4297,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" zoomScale="75" workbookViewId="0">
       <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Smooth edges and calculate the SSIM value for smoothed result
</commit_message>
<xml_diff>
--- a/Experiments/MakeGraph.xlsx
+++ b/Experiments/MakeGraph.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t>SSIM</t>
   </si>
@@ -39,13 +39,7 @@
     <t>head720_cells30_60</t>
   </si>
   <si>
-    <t>head720_cells30_55</t>
-  </si>
-  <si>
     <t>head720_cells30_50</t>
-  </si>
-  <si>
-    <t>head720_cells30_45</t>
   </si>
   <si>
     <t>head720_cells30_40</t>
@@ -58,12 +52,6 @@
   </si>
   <si>
     <t>head720_cells20_30</t>
-  </si>
-  <si>
-    <t>head720_cells20_25</t>
-  </si>
-  <si>
-    <t>head720_cells20_20</t>
   </si>
   <si>
     <t>head1080_cells20_40</t>
@@ -114,16 +102,19 @@
     <t>head720_cells5_8</t>
   </si>
   <si>
-    <t>head720_cells30_65</t>
-  </si>
-  <si>
     <t>head720_cells30_70</t>
   </si>
   <si>
-    <t>head720_cells30_75</t>
+    <t>head720_cells30_80</t>
   </si>
   <si>
-    <t>head720_cells30_80</t>
+    <t>head720_cells20_45</t>
+  </si>
+  <si>
+    <t>head720_cells20_50</t>
+  </si>
+  <si>
+    <t>head720_cells20_55</t>
   </si>
 </sst>
 </file>
@@ -415,12 +406,6 @@
                 <c:pt idx="2">
                   <c:v>0.953</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.945</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.934</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -438,12 +423,6 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>11.2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>11.9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -483,23 +462,17 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$6:$B$10</c:f>
+              <c:f>Sheet1!$B$4:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0.949</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.945</c:v>
+                  <c:v>0.941</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.941</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.936</c:v>
-                </c:pt>
-                <c:pt idx="4">
                   <c:v>0.929</c:v>
                 </c:pt>
               </c:numCache>
@@ -507,23 +480,17 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$6:$C$10</c:f>
+              <c:f>Sheet1!$C$4:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>13.3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.8</c:v>
+                  <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>15.1</c:v>
-                </c:pt>
-                <c:pt idx="4">
                   <c:v>15.7</c:v>
                 </c:pt>
               </c:numCache>
@@ -619,11 +586,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-594085056"/>
-        <c:axId val="-554766416"/>
+        <c:axId val="-560259328"/>
+        <c:axId val="-560684192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-594085056"/>
+        <c:axId val="-560259328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -729,12 +696,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-554766416"/>
+        <c:crossAx val="-560684192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-554766416"/>
+        <c:axId val="-560684192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -855,7 +822,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-594085056"/>
+        <c:crossAx val="-560259328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1225,23 +1192,17 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$6:$B$10</c:f>
+              <c:f>Sheet1!$B$4:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0.949</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.945</c:v>
+                  <c:v>0.941</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.941</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.936</c:v>
-                </c:pt>
-                <c:pt idx="4">
                   <c:v>0.929</c:v>
                 </c:pt>
               </c:numCache>
@@ -1249,23 +1210,17 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$6:$C$10</c:f>
+              <c:f>Sheet1!$C$4:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>13.3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.8</c:v>
+                  <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>15.1</c:v>
-                </c:pt>
-                <c:pt idx="4">
                   <c:v>15.7</c:v>
                 </c:pt>
               </c:numCache>
@@ -1282,11 +1237,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-594563584"/>
-        <c:axId val="-594561040"/>
+        <c:axId val="-460677760"/>
+        <c:axId val="-461083648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-594563584"/>
+        <c:axId val="-460677760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1391,12 +1346,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-594561040"/>
+        <c:crossAx val="-461083648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-594561040"/>
+        <c:axId val="-461083648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -1516,7 +1471,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-594563584"/>
+        <c:crossAx val="-460677760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2823,41 +2778,6 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.25501</cdr:x>
-      <cdr:y>0.24402</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.28328</cdr:x>
-      <cdr:y>0.27027</cdr:y>
-    </cdr:to>
-    <cdr:sp macro="" textlink="">
-      <cdr:nvSpPr>
-        <cdr:cNvPr id="5" name="TextBox 4"/>
-        <cdr:cNvSpPr txBox="1"/>
-      </cdr:nvSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="3299743" y="1794369"/>
-          <a:ext cx="365760" cy="193040"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </cdr:spPr>
-      <cdr:txBody>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>45</a:t>
-          </a:r>
-        </a:p>
-      </cdr:txBody>
-    </cdr:sp>
-  </cdr:relSizeAnchor>
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
       <cdr:x>0.32489</cdr:x>
       <cdr:y>0.27027</cdr:y>
     </cdr:from>
@@ -2886,41 +2806,6 @@
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
             <a:t>50</a:t>
-          </a:r>
-        </a:p>
-      </cdr:txBody>
-    </cdr:sp>
-  </cdr:relSizeAnchor>
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.37279</cdr:x>
-      <cdr:y>0.29928</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.39949</cdr:x>
-      <cdr:y>0.33106</cdr:y>
-    </cdr:to>
-    <cdr:sp macro="" textlink="">
-      <cdr:nvSpPr>
-        <cdr:cNvPr id="7" name="TextBox 6"/>
-        <cdr:cNvSpPr txBox="1"/>
-      </cdr:nvSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="4823743" y="2200769"/>
-          <a:ext cx="345440" cy="233680"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </cdr:spPr>
-      <cdr:txBody>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>55</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -2989,76 +2874,6 @@
         <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </cdr:txBody>
-    </cdr:sp>
-  </cdr:relSizeAnchor>
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.22441</cdr:x>
-      <cdr:y>0.33866</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.25622</cdr:x>
-      <cdr:y>0.36406</cdr:y>
-    </cdr:to>
-    <cdr:sp macro="" textlink="">
-      <cdr:nvSpPr>
-        <cdr:cNvPr id="10" name="TextBox 9"/>
-        <cdr:cNvSpPr txBox="1"/>
-      </cdr:nvSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="2921614" y="2503802"/>
-          <a:ext cx="414131" cy="187739"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </cdr:spPr>
-      <cdr:txBody>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>20</a:t>
-          </a:r>
-        </a:p>
-      </cdr:txBody>
-    </cdr:sp>
-  </cdr:relSizeAnchor>
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.37201</cdr:x>
-      <cdr:y>0.38123</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.40339</cdr:x>
-      <cdr:y>0.40887</cdr:y>
-    </cdr:to>
-    <cdr:sp macro="" textlink="">
-      <cdr:nvSpPr>
-        <cdr:cNvPr id="11" name="TextBox 10"/>
-        <cdr:cNvSpPr txBox="1"/>
-      </cdr:nvSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="4843179" y="2818541"/>
-          <a:ext cx="408609" cy="204304"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </cdr:spPr>
-      <cdr:txBody>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>25</a:t>
-          </a:r>
         </a:p>
       </cdr:txBody>
     </cdr:sp>
@@ -3855,8 +3670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="89" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A4" zoomScale="89" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3872,12 +3687,12 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D2">
         <v>80</v>
@@ -3885,112 +3700,83 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D3">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.94899999999999995</v>
+      </c>
+      <c r="C4">
+        <v>13.3</v>
       </c>
       <c r="D4">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="C5">
+        <v>14.5</v>
       </c>
       <c r="D5">
-        <v>65</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>0.94899999999999995</v>
+        <v>0.92900000000000005</v>
       </c>
       <c r="C6">
-        <v>13.3</v>
+        <v>15.7</v>
       </c>
       <c r="D6">
-        <v>60</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7">
-        <v>0.94499999999999995</v>
-      </c>
-      <c r="C7">
-        <v>13.8</v>
-      </c>
-      <c r="D7">
-        <v>55</v>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8">
-        <v>0.94099999999999995</v>
-      </c>
-      <c r="C8">
-        <v>14.5</v>
-      </c>
-      <c r="D8">
-        <v>50</v>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9">
-        <v>0.93600000000000005</v>
-      </c>
-      <c r="C9">
-        <v>15.1</v>
-      </c>
-      <c r="D9">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10">
-        <v>0.92900000000000005</v>
-      </c>
-      <c r="C10">
-        <v>15.7</v>
-      </c>
-      <c r="D10">
-        <v>40</v>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>17</v>
+      <c r="A15" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B16">
         <v>0.96299999999999997</v>
@@ -4004,7 +3790,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B17">
         <v>0.95899999999999996</v>
@@ -4018,7 +3804,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B18">
         <v>0.95299999999999996</v>
@@ -4028,34 +3814,6 @@
       </c>
       <c r="D18">
         <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19">
-        <v>0.94499999999999995</v>
-      </c>
-      <c r="C19">
-        <v>11.9</v>
-      </c>
-      <c r="D19">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20">
-        <v>0.93400000000000005</v>
-      </c>
-      <c r="C20">
-        <v>12.9</v>
-      </c>
-      <c r="D20">
-        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -4066,12 +3824,12 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B24">
         <v>0.97699999999999998</v>
@@ -4085,7 +3843,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B25">
         <v>0.97299999999999998</v>
@@ -4099,7 +3857,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B26">
         <v>0.96799999999999997</v>
@@ -4113,7 +3871,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B27">
         <v>0.96</v>
@@ -4127,7 +3885,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B28">
         <v>0.94599999999999995</v>
@@ -4147,12 +3905,12 @@
         <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C32">
         <v>7.28</v>
@@ -4163,7 +3921,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C33">
         <v>7.48</v>
@@ -4174,7 +3932,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C34">
         <v>7.29</v>
@@ -4185,7 +3943,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C35">
         <v>7.35</v>
@@ -4196,7 +3954,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C36">
         <v>7.33</v>
@@ -4213,12 +3971,12 @@
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B40">
         <v>0.97099999999999997</v>
@@ -4232,7 +3990,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B41">
         <v>0.96699999999999997</v>
@@ -4246,7 +4004,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B42">
         <v>0.96299999999999997</v>
@@ -4260,7 +4018,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B43">
         <v>0.95799999999999996</v>
@@ -4274,7 +4032,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B44">
         <v>0.95</v>

</xml_diff>

<commit_message>
Add poster and final version of dissertation
</commit_message>
<xml_diff>
--- a/Experiments/MakeGraph.xlsx
+++ b/Experiments/MakeGraph.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -895,11 +895,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1150270464"/>
-        <c:axId val="-1150266832"/>
+        <c:axId val="-1149418176"/>
+        <c:axId val="-1149414544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1150270464"/>
+        <c:axId val="-1149418176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1005,12 +1005,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1150266832"/>
+        <c:crossAx val="-1149414544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1150266832"/>
+        <c:axId val="-1149414544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -1131,7 +1131,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1150270464"/>
+        <c:crossAx val="-1149418176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1535,11 +1535,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1181499488"/>
-        <c:axId val="-1181496640"/>
+        <c:axId val="-1150568304"/>
+        <c:axId val="-1150564912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1181499488"/>
+        <c:axId val="-1150568304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1650,7 +1650,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1181496640"/>
+        <c:crossAx val="-1150564912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1658,7 +1658,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1181496640"/>
+        <c:axId val="-1150564912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1764,7 +1764,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1181499488"/>
+        <c:crossAx val="-1150568304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2114,11 +2114,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1157089680"/>
-        <c:axId val="-1157385168"/>
+        <c:axId val="-1150738720"/>
+        <c:axId val="-1150735328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1157089680"/>
+        <c:axId val="-1150738720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2224,7 +2224,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1157385168"/>
+        <c:crossAx val="-1150735328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2232,7 +2232,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1157385168"/>
+        <c:axId val="-1150735328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2337,7 +2337,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1157089680"/>
+        <c:crossAx val="-1150738720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2668,11 +2668,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1181466240"/>
-        <c:axId val="-1181432928"/>
+        <c:axId val="-1177128912"/>
+        <c:axId val="-1181325968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1181466240"/>
+        <c:axId val="-1177128912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2778,7 +2778,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1181432928"/>
+        <c:crossAx val="-1181325968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2786,7 +2786,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1181432928"/>
+        <c:axId val="-1181325968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2891,7 +2891,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1181466240"/>
+        <c:crossAx val="-1177128912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3026,6 +3026,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3283,11 +3284,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1181412224"/>
-        <c:axId val="-1181408832"/>
+        <c:axId val="-1151081968"/>
+        <c:axId val="-1151078576"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1181412224"/>
+        <c:axId val="-1151081968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3398,7 +3399,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1181408832"/>
+        <c:crossAx val="-1151078576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3406,7 +3407,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1181408832"/>
+        <c:axId val="-1151078576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3519,7 +3520,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1181412224"/>
+        <c:crossAx val="-1151081968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3533,6 +3534,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3639,6 +3641,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3896,11 +3899,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1150534784"/>
-        <c:axId val="-1150531392"/>
+        <c:axId val="-1181062352"/>
+        <c:axId val="-1181058960"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1150534784"/>
+        <c:axId val="-1181062352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4006,7 +4009,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1150531392"/>
+        <c:crossAx val="-1181058960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4014,7 +4017,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1150531392"/>
+        <c:axId val="-1181058960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4127,7 +4130,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1150534784"/>
+        <c:crossAx val="-1181062352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4231,9 +4234,87 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1200"/>
+              <a:t>Comparison between smoothed</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1200" baseline="0"/>
+              <a:t> and unsmoothed results</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1200"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.117096534691638"/>
+          <c:y val="0.028038858472574"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.165260333245942"/>
+          <c:y val="0.147904978442828"/>
+          <c:w val="0.792769977461946"/>
+          <c:h val="0.619473318376822"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -4370,16 +4451,80 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1157340928"/>
-        <c:axId val="-1157338608"/>
+        <c:axId val="-1149290880"/>
+        <c:axId val="-1149288560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1157340928"/>
+        <c:axId val="-1149290880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN"/>
+                  <a:t>NUmber of Components</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.39196186816891"/>
+              <c:y val="0.831392261790211"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4417,7 +4562,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1157338608"/>
+        <c:crossAx val="-1149288560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4425,7 +4570,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1157338608"/>
+        <c:axId val="-1149288560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4445,6 +4590,70 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN"/>
+                  <a:t>SSIM</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.0167878757168445"/>
+              <c:y val="0.412639269782758"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4475,7 +4684,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1157340928"/>
+        <c:crossAx val="-1149290880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4489,6 +4698,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.345758858248201"/>
+          <c:y val="0.897774443206041"/>
+          <c:w val="0.34765377319624"/>
+          <c:h val="0.0882061275576719"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4552,6 +4771,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -4718,11 +4938,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1150173120"/>
-        <c:axId val="-1150170272"/>
+        <c:axId val="-1149264864"/>
+        <c:axId val="-1149261472"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1150173120"/>
+        <c:axId val="-1149264864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4828,7 +5048,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1150170272"/>
+        <c:crossAx val="-1149261472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4836,7 +5056,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1150170272"/>
+        <c:axId val="-1149261472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4949,7 +5169,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1150173120"/>
+        <c:crossAx val="-1149264864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5572,11 +5792,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1181549424"/>
-        <c:axId val="-1176968736"/>
+        <c:axId val="-1150766480"/>
+        <c:axId val="-1150817536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1181549424"/>
+        <c:axId val="-1150766480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5664,12 +5884,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1176968736"/>
+        <c:crossAx val="-1150817536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1176968736"/>
+        <c:axId val="-1150817536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="17.0"/>
@@ -5787,7 +6007,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1181549424"/>
+        <c:crossAx val="-1150766480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6312,11 +6532,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1175545216"/>
-        <c:axId val="-1177706752"/>
+        <c:axId val="-1150354112"/>
+        <c:axId val="-1150336928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1175545216"/>
+        <c:axId val="-1150354112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6432,12 +6652,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1177706752"/>
+        <c:crossAx val="-1150336928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1177706752"/>
+        <c:axId val="-1150336928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6548,7 +6768,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1175545216"/>
+        <c:crossAx val="-1150354112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7061,11 +7281,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1179079904"/>
-        <c:axId val="-1179076272"/>
+        <c:axId val="-1150393296"/>
+        <c:axId val="-1150389664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1179079904"/>
+        <c:axId val="-1150393296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7177,12 +7397,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1179076272"/>
+        <c:crossAx val="-1150389664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1179076272"/>
+        <c:axId val="-1150389664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="17.0"/>
@@ -7309,7 +7529,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1179079904"/>
+        <c:crossAx val="-1150393296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7438,6 +7658,17 @@
               <a:rPr lang="en-US" sz="1400" b="1" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
+              <a:t>Relationship among memory cost, frame rate and result quality</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
               <a:t>(Figures shown are the number of eigenvectors)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" sz="1400">
@@ -7446,7 +7677,14 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.213160756504348"/>
+          <c:y val="0.0128233063491926"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7483,10 +7721,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.103926462857108"/>
+          <c:x val="0.0884658736835877"/>
           <c:y val="0.122028889326953"/>
-          <c:w val="0.845766810573195"/>
-          <c:h val="0.642726608828149"/>
+          <c:w val="0.882872132787191"/>
+          <c:h val="0.691455093891845"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -7734,11 +7972,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1150244224"/>
-        <c:axId val="-1150241520"/>
+        <c:axId val="-1149381520"/>
+        <c:axId val="-1149379392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1150244224"/>
+        <c:axId val="-1149381520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7784,7 +8022,14 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.451942164963351"/>
+              <c:y val="0.87828440720278"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7851,12 +8096,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1150241520"/>
+        <c:crossAx val="-1149379392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1150241520"/>
+        <c:axId val="-1149379392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="3.0"/>
@@ -7903,7 +8148,14 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.020527077411109"/>
+              <c:y val="0.493108028177348"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7970,7 +8222,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1150244224"/>
+        <c:crossAx val="-1149381520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7984,7 +8236,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.169919119524127"/>
+          <c:y val="0.937689837943699"/>
+          <c:w val="0.666345850558533"/>
+          <c:h val="0.0546161782467854"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8066,9 +8327,80 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Reconstruction</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> comparison between normal CPU and CUDA</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.093163947958676"/>
+          <c:y val="0.106782744282744"/>
+          <c:w val="0.887422003329711"/>
+          <c:h val="0.729687576734821"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -8205,11 +8537,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1181248944"/>
-        <c:axId val="-1181246400"/>
+        <c:axId val="-1149329136"/>
+        <c:axId val="-1149325744"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1181248944"/>
+        <c:axId val="-1149329136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8222,7 +8554,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -8235,17 +8567,25 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1100"/>
+                  <a:rPr lang="en-US" sz="1200"/>
                   <a:t>Number</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1100" baseline="0"/>
+                  <a:rPr lang="en-US" sz="1200" baseline="0"/>
                   <a:t> of components used in PCA</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US" sz="1100"/>
+                <a:endParaRPr lang="en-US" sz="1200"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.378275443243438"/>
+              <c:y val="0.881723198061781"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -8259,7 +8599,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -8312,7 +8652,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1181246400"/>
+        <c:crossAx val="-1149325744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8320,7 +8660,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1181246400"/>
+        <c:axId val="-1149325744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8361,7 +8701,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -8374,12 +8714,13 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1100"/>
+                  <a:rPr lang="en-US" sz="1200"/>
                   <a:t>FPS</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -8393,7 +8734,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -8440,7 +8781,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1181248944"/>
+        <c:crossAx val="-1149329136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8454,6 +8795,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.295945284901512"/>
+          <c:y val="0.929618208456791"/>
+          <c:w val="0.446937388650633"/>
+          <c:h val="0.0521905233519407"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8534,9 +8885,80 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Reconstruction comparison</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> between normal CPU and GPU (OpenCL)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.157547745337105"/>
+          <c:y val="0.211917605624388"/>
+          <c:w val="0.813761100142581"/>
+          <c:h val="0.593748407870009"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
@@ -8605,11 +9027,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="-1151196752"/>
-        <c:axId val="-1181596416"/>
+        <c:axId val="-1150382576"/>
+        <c:axId val="-1181292816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1151196752"/>
+        <c:axId val="-1150382576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8622,7 +9044,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -8635,17 +9057,25 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1200"/>
                   <a:t>Cells</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:rPr lang="en-US" sz="1200" baseline="0"/>
                   <a:t> Dimension</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="en-US" sz="1200"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.0139548416927597"/>
+              <c:y val="0.315195668033354"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -8659,7 +9089,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -8712,7 +9142,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1181596416"/>
+        <c:crossAx val="-1181292816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8720,7 +9150,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1181596416"/>
+        <c:axId val="-1181292816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8747,7 +9177,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -8760,14 +9190,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1200"/>
                   <a:t>Average</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:rPr lang="en-US" sz="1200" baseline="0"/>
                   <a:t> FPS(GPU)/FPS(only_CPU)</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="en-US" sz="1200"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -8792,7 +9222,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -8838,7 +9268,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1151196752"/>
+        <c:crossAx val="-1150382576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9171,11 +9601,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1175627808"/>
-        <c:axId val="-1175137360"/>
+        <c:axId val="-1150764080"/>
+        <c:axId val="-1150760688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1175627808"/>
+        <c:axId val="-1150764080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9286,7 +9716,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1175137360"/>
+        <c:crossAx val="-1150760688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9294,7 +9724,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1175137360"/>
+        <c:axId val="-1150760688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9407,7 +9837,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1175627808"/>
+        <c:crossAx val="-1150764080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9532,6 +9962,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9789,11 +10220,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1157087584"/>
-        <c:axId val="-1157084464"/>
+        <c:axId val="-1150458304"/>
+        <c:axId val="-1150454912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1157087584"/>
+        <c:axId val="-1150458304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9904,7 +10335,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1157084464"/>
+        <c:crossAx val="-1150454912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9912,7 +10343,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1157084464"/>
+        <c:axId val="-1150454912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10025,7 +10456,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1157087584"/>
+        <c:crossAx val="-1150458304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18955,16 +19386,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1270000</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>168611</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>6483</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>689041</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>607977</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>54043</xdr:rowOff>
+      <xdr:rowOff>94575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -18987,6 +19418,308 @@
 </file>
 
 <file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.21918</cdr:x>
+      <cdr:y>0.32472</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.45284</cdr:x>
+      <cdr:y>0.428</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="994871" y="882482"/>
+          <a:ext cx="1060546" cy="280667"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>10*10 cells</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.49155</cdr:x>
+      <cdr:y>0.35367</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.8137</cdr:x>
+      <cdr:y>0.45694</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 2"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2231154" y="961154"/>
+          <a:ext cx="1462204" cy="280639"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>20*20 cells</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.75402</cdr:x>
+      <cdr:y>0.12622</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.93946</cdr:x>
+      <cdr:y>0.22948</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="TextBox 3"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3422481" y="343012"/>
+          <a:ext cx="841696" cy="280640"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>30*30 cells</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
@@ -25866,15 +26599,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>335280</xdr:colOff>
+      <xdr:colOff>347980</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>162560</xdr:rowOff>
+      <xdr:rowOff>149860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
+      <xdr:colOff>114300</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>172720</xdr:rowOff>
+      <xdr:rowOff>160020</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -25900,16 +26633,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>160828</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>31135</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>707064</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>3822</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>614446</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>135750</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>791972</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>108438</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -26478,7 +27211,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A12" zoomScale="94" zoomScaleNormal="91" zoomScalePageLayoutView="91" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="A12" zoomScale="94" zoomScaleNormal="91" zoomScalePageLayoutView="91" workbookViewId="0">
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
@@ -27484,7 +28217,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScale="125" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -27564,7 +28297,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="B1" zoomScale="135" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" zoomScale="93" workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -28774,7 +29507,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView showRuler="0" zoomScale="113" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>